<commit_message>
Corrected Sullivan Smith's V40 10000m time in club records source sheet, was a smidge low hence runbritain result was not being listed alongside it
</commit_message>
<xml_diff>
--- a/2022_CnC_records.xlsx
+++ b/2022_CnC_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1246FCF0-4B26-4205-A9A2-949A425E8445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A470B970-1C48-4D9A-8D95-F6F73DE2C09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="2022_Overall" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4576" uniqueCount="1188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4577" uniqueCount="1189">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2967,9 +2967,6 @@
     <t xml:space="preserve">15:23.2 </t>
   </si>
   <si>
-    <t xml:space="preserve">32:06.3 </t>
-  </si>
-  <si>
     <t xml:space="preserve">4:39.5 </t>
   </si>
   <si>
@@ -3607,6 +3604,12 @@
   </si>
   <si>
     <t>Carole Morris</t>
+  </si>
+  <si>
+    <t>Corrected from original 32:06.3 to powerof10 time</t>
+  </si>
+  <si>
+    <t>32:06.62</t>
   </si>
 </sst>
 </file>
@@ -4011,7 +4014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0672E4C-1F81-4344-8F80-ED5988EB27BD}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -4026,7 +4029,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>379</v>
@@ -4055,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -4602,7 +4605,7 @@
         <v>38</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>98</v>
@@ -4689,7 +4692,7 @@
     </row>
     <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
@@ -9795,7 +9798,7 @@
         <v>667</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>101</v>
@@ -9818,7 +9821,7 @@
         <v>668</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>100</v>
@@ -14325,8 +14328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA3259E-AFD6-4FCB-BD83-44E5FC56E958}">
   <dimension ref="A1:J229"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="G229" sqref="G229"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14587,7 +14590,7 @@
         <v>919</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>98</v>
@@ -14596,7 +14599,7 @@
         <v>888</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -14935,7 +14938,7 @@
         <v>38</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>98</v>
@@ -15018,7 +15021,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>1</v>
@@ -15185,7 +15188,7 @@
         <v>624</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>974</v>
+        <v>1188</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>299</v>
@@ -15201,6 +15204,9 @@
       </c>
       <c r="I38" s="1" t="s">
         <v>889</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>1187</v>
       </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.2">
@@ -15208,7 +15214,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>299</v>
@@ -15231,7 +15237,7 @@
         <v>957</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>703</v>
@@ -15240,7 +15246,7 @@
         <v>958</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>98</v>
@@ -15249,7 +15255,7 @@
         <v>889</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.2">
@@ -15257,7 +15263,7 @@
         <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>646</v>
@@ -15280,7 +15286,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>299</v>
@@ -15303,7 +15309,7 @@
         <v>20</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>299</v>
@@ -15326,7 +15332,7 @@
         <v>60</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>486</v>
@@ -15349,7 +15355,7 @@
         <v>62</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>667</v>
@@ -15372,7 +15378,7 @@
         <v>64</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>703</v>
@@ -15395,7 +15401,7 @@
         <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>703</v>
@@ -15418,7 +15424,7 @@
         <v>921</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>674</v>
@@ -15441,7 +15447,7 @@
         <v>923</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>674</v>
@@ -15464,7 +15470,7 @@
         <v>960</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>530</v>
@@ -15487,7 +15493,7 @@
         <v>925</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>701</v>
@@ -15588,7 +15594,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>98</v>
@@ -15625,7 +15631,7 @@
         <v>642</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>486</v>
@@ -15648,7 +15654,7 @@
         <v>644</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>486</v>
@@ -15668,19 +15674,19 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>378</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>388</v>
@@ -15697,13 +15703,13 @@
         <v>3</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>378</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>383</v>
@@ -15720,13 +15726,13 @@
         <v>5</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>1003</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>1004</v>
-      </c>
       <c r="F62" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>384</v>
@@ -15743,13 +15749,13 @@
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>385</v>
@@ -15766,13 +15772,13 @@
         <v>9</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>530</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>386</v>
@@ -15789,13 +15795,13 @@
         <v>11</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>703</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>387</v>
@@ -15812,13 +15818,13 @@
         <v>12</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>703</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>601</v>
@@ -15835,13 +15841,13 @@
         <v>624</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>1009</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>1010</v>
-      </c>
       <c r="F67" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>899</v>
@@ -15858,13 +15864,13 @@
         <v>14</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>674</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>80</v>
@@ -15881,7 +15887,7 @@
         <v>957</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>667</v>
@@ -15890,7 +15896,7 @@
         <v>958</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>98</v>
@@ -15899,7 +15905,7 @@
         <v>890</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.2">
@@ -15907,7 +15913,7 @@
         <v>55</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>801</v>
@@ -15927,7 +15933,7 @@
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C71" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>0</v>
@@ -15953,7 +15959,7 @@
         <v>20</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>351</v>
@@ -15976,13 +15982,13 @@
         <v>60</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>423</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>85</v>
@@ -15999,13 +16005,13 @@
         <v>62</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>378</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>86</v>
@@ -16022,13 +16028,13 @@
         <v>64</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>423</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>87</v>
@@ -16045,7 +16051,7 @@
         <v>66</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>740</v>
@@ -16068,7 +16074,7 @@
         <v>921</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>653</v>
@@ -16091,13 +16097,13 @@
         <v>923</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>801</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>110</v>
@@ -16114,13 +16120,13 @@
         <v>960</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>801</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>103</v>
@@ -16137,7 +16143,7 @@
         <v>925</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>653</v>
@@ -16160,13 +16166,13 @@
         <v>636</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>671</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>902</v>
@@ -16206,13 +16212,13 @@
         <v>681</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>671</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>900</v>
@@ -16295,13 +16301,13 @@
         <v>644</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>653</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>106</v>
@@ -16315,19 +16321,19 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>674</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>388</v>
@@ -16344,13 +16350,13 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>674</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>383</v>
@@ -16367,13 +16373,13 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>674</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>384</v>
@@ -16390,13 +16396,13 @@
         <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>1044</v>
-      </c>
       <c r="F92" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>385</v>
@@ -16413,13 +16419,13 @@
         <v>9</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>721</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>386</v>
@@ -16436,13 +16442,13 @@
         <v>11</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>721</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>387</v>
@@ -16459,13 +16465,13 @@
         <v>12</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>674</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>601</v>
@@ -16482,13 +16488,13 @@
         <v>14</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>674</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>80</v>
@@ -16502,10 +16508,10 @@
     </row>
     <row r="97" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C97" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>740</v>
@@ -16514,7 +16520,7 @@
         <v>958</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>98</v>
@@ -16528,7 +16534,7 @@
         <v>55</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>801</v>
@@ -16551,13 +16557,13 @@
         <v>60</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E99" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>1028</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>1029</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>85</v>
@@ -16574,13 +16580,13 @@
         <v>62</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>674</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>86</v>
@@ -16597,13 +16603,13 @@
         <v>64</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>659</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>87</v>
@@ -16620,13 +16626,13 @@
         <v>66</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E102" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>1030</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>1031</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>88</v>
@@ -16640,16 +16646,16 @@
     </row>
     <row r="103" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C103" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>701</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>602</v>
@@ -16663,16 +16669,16 @@
     </row>
     <row r="104" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C104" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>617</v>
@@ -16686,16 +16692,16 @@
     </row>
     <row r="105" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C105" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>701</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>608</v>
@@ -16709,10 +16715,10 @@
     </row>
     <row r="106" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C106" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>526</v>
@@ -16735,13 +16741,13 @@
         <v>636</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>764</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>902</v>
@@ -16758,13 +16764,13 @@
         <v>638</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>734</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>901</v>
@@ -16781,13 +16787,13 @@
         <v>681</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>734</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>900</v>
@@ -16847,13 +16853,13 @@
         <v>642</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>486</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>105</v>
@@ -16870,13 +16876,13 @@
         <v>644</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>734</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>106</v>
@@ -16890,13 +16896,13 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>701</v>
@@ -16919,7 +16925,7 @@
         <v>3</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>774</v>
@@ -16942,13 +16948,13 @@
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>384</v>
@@ -16965,13 +16971,13 @@
         <v>7</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>385</v>
@@ -16988,13 +16994,13 @@
         <v>9</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>386</v>
@@ -17011,13 +17017,13 @@
         <v>11</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>486</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>387</v>
@@ -17034,13 +17040,13 @@
         <v>12</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>601</v>
@@ -17057,13 +17063,13 @@
         <v>14</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>486</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>80</v>
@@ -17077,19 +17083,19 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C123" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>351</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>98</v>
@@ -17106,13 +17112,13 @@
         <v>55</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>82</v>
@@ -17129,13 +17135,13 @@
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>85</v>
@@ -17152,13 +17158,13 @@
         <v>62</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>299</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>86</v>
@@ -17175,13 +17181,13 @@
         <v>64</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>653</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>87</v>
@@ -17198,7 +17204,7 @@
         <v>66</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>774</v>
@@ -17218,16 +17224,16 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C129" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>299</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>602</v>
@@ -17241,16 +17247,16 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C130" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>617</v>
@@ -17264,16 +17270,16 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C131" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>742</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>608</v>
@@ -17287,7 +17293,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C132" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>700</v>
@@ -17296,7 +17302,7 @@
         <v>328</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>615</v>
@@ -17310,19 +17316,19 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C133" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>371</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>98</v>
@@ -17339,13 +17345,13 @@
         <v>636</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>653</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>902</v>
@@ -17362,13 +17368,13 @@
         <v>638</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>299</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>901</v>
@@ -17385,13 +17391,13 @@
         <v>681</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>299</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>900</v>
@@ -17405,19 +17411,19 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C137" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D137" s="1" t="s">
         <v>1072</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>1073</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>594</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>98</v>
@@ -17428,16 +17434,16 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C138" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>1074</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>1075</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>671</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>98</v>
@@ -17446,7 +17452,7 @@
         <v>892</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
@@ -17497,7 +17503,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>1</v>
@@ -17509,7 +17515,7 @@
         <v>526</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>388</v>
@@ -17526,7 +17532,7 @@
         <v>3</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>742</v>
@@ -17549,13 +17555,13 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>667</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>384</v>
@@ -17572,13 +17578,13 @@
         <v>7</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>667</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>385</v>
@@ -17595,13 +17601,13 @@
         <v>9</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>386</v>
@@ -17618,13 +17624,13 @@
         <v>11</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>387</v>
@@ -17641,13 +17647,13 @@
         <v>12</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>601</v>
@@ -17664,13 +17670,13 @@
         <v>624</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>899</v>
@@ -17687,13 +17693,13 @@
         <v>14</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>351</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>80</v>
@@ -17707,7 +17713,7 @@
     </row>
     <row r="151" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C151" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>0</v>
@@ -17753,13 +17759,13 @@
         <v>60</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>85</v>
@@ -17776,13 +17782,13 @@
         <v>62</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>351</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>86</v>
@@ -17799,13 +17805,13 @@
         <v>64</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>87</v>
@@ -17822,7 +17828,7 @@
         <v>66</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>742</v>
@@ -17842,16 +17848,16 @@
     </row>
     <row r="157" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C157" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>351</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>616</v>
@@ -17868,13 +17874,13 @@
         <v>631</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>659</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>109</v>
@@ -17891,13 +17897,13 @@
         <v>716</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>659</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>100</v>
@@ -17911,19 +17917,19 @@
     </row>
     <row r="160" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C160" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>378</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>98</v>
@@ -17934,19 +17940,19 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C161" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>378</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>98</v>
@@ -17963,13 +17969,13 @@
         <v>636</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>671</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G162" s="1" t="s">
         <v>902</v>
@@ -18009,13 +18015,13 @@
         <v>681</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>671</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>900</v>
@@ -18029,19 +18035,19 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C165" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>378</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="H165" s="1" t="s">
         <v>98</v>
@@ -18052,16 +18058,16 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C166" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>378</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>98</v>
@@ -18070,7 +18076,7 @@
         <v>893</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
@@ -18121,13 +18127,13 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>378</v>
@@ -18150,7 +18156,7 @@
         <v>3</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>378</v>
@@ -18173,7 +18179,7 @@
         <v>5</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>378</v>
@@ -18196,13 +18202,13 @@
         <v>7</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>486</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="G173" s="1" t="s">
         <v>385</v>
@@ -18219,13 +18225,13 @@
         <v>9</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>423</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>386</v>
@@ -18242,13 +18248,13 @@
         <v>11</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>486</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>387</v>
@@ -18302,7 +18308,7 @@
     </row>
     <row r="178" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C178" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>0</v>
@@ -18345,7 +18351,7 @@
         <v>60</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>378</v>
@@ -18368,7 +18374,7 @@
         <v>62</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>378</v>
@@ -18391,7 +18397,7 @@
         <v>64</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>674</v>
@@ -18414,7 +18420,7 @@
         <v>66</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>674</v>
@@ -18434,16 +18440,16 @@
     </row>
     <row r="184" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C184" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="G184" s="1" t="s">
         <v>616</v>
@@ -18460,13 +18466,13 @@
         <v>631</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>109</v>
@@ -18483,7 +18489,7 @@
         <v>716</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>423</v>
@@ -18503,19 +18509,19 @@
     </row>
     <row r="187" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C187" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="H187" s="1" t="s">
         <v>98</v>
@@ -18526,7 +18532,7 @@
     </row>
     <row r="188" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C188" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>0</v>
@@ -18549,13 +18555,13 @@
         <v>636</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>902</v>
@@ -18572,13 +18578,13 @@
         <v>638</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>901</v>
@@ -18595,13 +18601,13 @@
         <v>681</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>900</v>
@@ -18615,7 +18621,7 @@
     </row>
     <row r="192" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C192" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>0</v>
@@ -18635,7 +18641,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C193" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>0</v>
@@ -18695,13 +18701,13 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>764</v>
@@ -18724,7 +18730,7 @@
         <v>3</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>653</v>
@@ -18747,7 +18753,7 @@
         <v>5</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>764</v>
@@ -18770,13 +18776,13 @@
         <v>7</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>742</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G200" s="1" t="s">
         <v>385</v>
@@ -18793,13 +18799,13 @@
         <v>9</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>832</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G201" s="1" t="s">
         <v>386</v>
@@ -18839,13 +18845,13 @@
         <v>12</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G203" s="1" t="s">
         <v>601</v>
@@ -18862,13 +18868,13 @@
         <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>653</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>80</v>
@@ -18931,7 +18937,7 @@
         <v>64</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>764</v>
@@ -18954,7 +18960,7 @@
         <v>66</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>764</v>
@@ -18997,13 +19003,13 @@
         <v>631</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>734</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>109</v>
@@ -19020,13 +19026,13 @@
         <v>752</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>299</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G211" s="1" t="s">
         <v>404</v>
@@ -19043,13 +19049,13 @@
         <v>634</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>653</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G212" s="1" t="s">
         <v>107</v>
@@ -19063,7 +19069,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C213" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>0</v>
@@ -19106,13 +19112,13 @@
         <v>638</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>423</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>901</v>
@@ -19129,13 +19135,13 @@
         <v>681</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>486</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>900</v>
@@ -19149,7 +19155,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>1</v>
@@ -19235,13 +19241,13 @@
         <v>9</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>671</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>386</v>
@@ -19358,13 +19364,13 @@
         <v>752</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>526</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="G228" s="1" t="s">
         <v>404</v>

</xml_diff>

<commit_message>
Starting to work through 2009 club records
</commit_message>
<xml_diff>
--- a/2022_CnC_records.xlsx
+++ b/2022_CnC_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284D3815-B752-4A5D-962E-BF5A445EBC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7CB7FC-B25C-4A8F-9FD7-DD8374CF2FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4576" uniqueCount="1191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4578" uniqueCount="1191">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -4020,8 +4020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0672E4C-1F81-4344-8F80-ED5988EB27BD}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4969,7 +4969,7 @@
         <v>58</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>92</v>
+        <v>395</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>99</v>
@@ -4992,7 +4992,7 @@
         <v>59</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>83</v>
+        <v>905</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>99</v>
@@ -5300,8 +5300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E116B990-5FBC-4F60-A519-6D8AF60704F6}">
   <dimension ref="A2:J100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6721,6 +6721,9 @@
       <c r="I68" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="J68" s="1" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C69" s="1" t="s">
@@ -6769,6 +6772,9 @@
       </c>
       <c r="I70" s="1" t="s">
         <v>390</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -7335,8 +7341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33EFF66-21E6-4C12-9015-9A2807500A5E}">
   <dimension ref="A2:K88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:I2"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14331,8 +14337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA3259E-AFD6-4FCB-BD83-44E5FC56E958}">
   <dimension ref="A1:J229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Worked a little further through 2009 records
</commit_message>
<xml_diff>
--- a/2022_CnC_records.xlsx
+++ b/2022_CnC_records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7CB7FC-B25C-4A8F-9FD7-DD8374CF2FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCA3534-F465-4FE8-AAF5-A397BCF4CE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
+    <workbookView xWindow="14475" yWindow="2685" windowWidth="23160" windowHeight="13305" activeTab="1" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -5300,8 +5300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E116B990-5FBC-4F60-A519-6D8AF60704F6}">
   <dimension ref="A2:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9322,9 +9322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC38CDD-B783-4755-B4DD-3225A4BF53C5}">
   <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="J125" sqref="J125"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14337,8 +14335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA3259E-AFD6-4FCB-BD83-44E5FC56E958}">
   <dimension ref="A1:J229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="J138" sqref="J138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Completed 2021 records. Some age group javelin weights might still be iffy
</commit_message>
<xml_diff>
--- a/2022_CnC_records.xlsx
+++ b/2022_CnC_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A763E7EC-35FB-4E2A-92E5-393CFF2EC6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787FA52D-122F-4E68-BCAC-58909E7E1C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4578" uniqueCount="1191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4513" uniqueCount="1188">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2751,24 +2751,12 @@
     <t>HepW</t>
   </si>
   <si>
-    <t>80HW</t>
-  </si>
-  <si>
-    <t>300H</t>
-  </si>
-  <si>
     <t>2000SCW</t>
   </si>
   <si>
     <t>Checked Po10 for hammer weight</t>
   </si>
   <si>
-    <t>SP2K</t>
-  </si>
-  <si>
-    <t>HT2K</t>
-  </si>
-  <si>
     <t>1500W</t>
   </si>
   <si>
@@ -3579,12 +3567,6 @@
     <t>110HM35</t>
   </si>
   <si>
-    <t>TODO event code may well be wrong</t>
-  </si>
-  <si>
-    <t>Po10 has this event code, gets used for next couple of AGs</t>
-  </si>
-  <si>
     <t xml:space="preserve">C&amp;C AC Track and Field records  - Overall club records </t>
   </si>
   <si>
@@ -3616,6 +3598,15 @@
   </si>
   <si>
     <t>Age Code</t>
+  </si>
+  <si>
+    <t>80HW40</t>
+  </si>
+  <si>
+    <t>80HW50</t>
+  </si>
+  <si>
+    <t>75HU13M</t>
   </si>
 </sst>
 </file>
@@ -4021,7 +4012,7 @@
   <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4035,7 +4026,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>1180</v>
+        <v>1174</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>378</v>
@@ -4056,7 +4047,7 @@
         <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1190</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -4064,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1181</v>
+        <v>1175</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -4611,7 +4602,7 @@
         <v>38</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>97</v>
@@ -4698,7 +4689,7 @@
     </row>
     <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>1182</v>
+        <v>1176</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
@@ -4992,7 +4983,7 @@
         <v>59</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>98</v>
@@ -5301,7 +5292,7 @@
   <dimension ref="A2:J100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5338,7 +5329,7 @@
         <v>95</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>1190</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5491,15 +5482,6 @@
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -7341,8 +7323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33EFF66-21E6-4C12-9015-9A2807500A5E}">
   <dimension ref="A2:K88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7375,7 +7357,7 @@
         <v>95</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>1190</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -9021,7 +9003,7 @@
         <v>441</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>80</v>
+        <v>1187</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>97</v>
@@ -9323,7 +9305,7 @@
   <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9356,7 +9338,7 @@
         <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1190</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -9652,7 +9634,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>98</v>
@@ -9810,7 +9792,7 @@
         <v>666</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1184</v>
+        <v>1178</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>100</v>
@@ -9833,7 +9815,7 @@
         <v>667</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>99</v>
@@ -10250,7 +10232,7 @@
         <v>628</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>902</v>
+        <v>1185</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>98</v>
@@ -10319,7 +10301,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>98</v>
@@ -10894,7 +10876,7 @@
         <v>628</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>902</v>
+        <v>1185</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>98</v>
@@ -10963,7 +10945,7 @@
         <v>0</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>98</v>
@@ -11538,7 +11520,7 @@
         <v>747</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>902</v>
+        <v>1186</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>98</v>
@@ -11607,7 +11589,7 @@
         <v>708</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>98</v>
@@ -12069,22 +12051,13 @@
       <c r="F123" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G123" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="H123" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I123" s="1" t="s">
-        <v>890</v>
-      </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C124" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1188</v>
+        <v>1182</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>652</v>
@@ -12102,7 +12075,7 @@
         <v>890</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>1189</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
@@ -12118,15 +12091,6 @@
       <c r="F125" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G125" s="1" t="s">
-        <v>902</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>890</v>
-      </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C126" s="1" t="s">
@@ -12141,15 +12105,6 @@
       <c r="F126" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G126" s="1" t="s">
-        <v>903</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I126" s="1" t="s">
-        <v>890</v>
-      </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C127" s="1" t="s">
@@ -12188,7 +12143,7 @@
         <v>708</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>98</v>
@@ -12279,15 +12234,6 @@
       <c r="F132" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G132" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H132" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I132" s="1" t="s">
-        <v>890</v>
-      </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C133" s="1" t="s">
@@ -12441,7 +12387,7 @@
         <v>708</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>1187</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
@@ -12644,15 +12590,6 @@
       <c r="F149" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G149" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I149" s="1" t="s">
-        <v>891</v>
-      </c>
     </row>
     <row r="150" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C150" s="1" t="s">
@@ -12713,15 +12650,6 @@
       <c r="F152" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G152" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H152" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I152" s="1" t="s">
-        <v>891</v>
-      </c>
     </row>
     <row r="153" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C153" s="1" t="s">
@@ -13107,15 +13035,6 @@
       <c r="F170" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G170" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H170" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I170" s="1" t="s">
-        <v>892</v>
-      </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C171" s="1" t="s">
@@ -13340,15 +13259,6 @@
       <c r="F181" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G181" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="H181" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I181" s="1" t="s">
-        <v>893</v>
-      </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C182" s="1" t="s">
@@ -13363,15 +13273,6 @@
       <c r="F182" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G182" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="H182" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I182" s="1" t="s">
-        <v>893</v>
-      </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C183" s="1" t="s">
@@ -13386,15 +13287,6 @@
       <c r="F183" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G183" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H183" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I183" s="1" t="s">
-        <v>893</v>
-      </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C184" s="1" t="s">
@@ -13488,7 +13380,7 @@
         <v>893</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
@@ -13660,7 +13552,7 @@
         <v>9</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>485</v>
@@ -13714,15 +13606,6 @@
       <c r="F198" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G198" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H198" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I198" s="1" t="s">
-        <v>894</v>
-      </c>
     </row>
     <row r="199" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C199" s="1" t="s">
@@ -13760,15 +13643,6 @@
       <c r="F200" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G200" s="1" t="s">
-        <v>906</v>
-      </c>
-      <c r="H200" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I200" s="1" t="s">
-        <v>894</v>
-      </c>
     </row>
     <row r="201" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C201" s="1" t="s">
@@ -13806,15 +13680,6 @@
       <c r="F202" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G202" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="H202" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I202" s="1" t="s">
-        <v>894</v>
-      </c>
     </row>
     <row r="203" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C203" s="1" t="s">
@@ -13875,15 +13740,6 @@
       <c r="F205" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G205" s="1" t="s">
-        <v>907</v>
-      </c>
-      <c r="H205" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I205" s="1" t="s">
-        <v>894</v>
-      </c>
     </row>
     <row r="206" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C206" s="1" t="s">
@@ -13899,7 +13755,7 @@
         <v>783</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>98</v>
@@ -14131,15 +13987,6 @@
       <c r="F217" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G217" s="1" t="s">
-        <v>906</v>
-      </c>
-      <c r="H217" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I217" s="1" t="s">
-        <v>895</v>
-      </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C218" s="1" t="s">
@@ -14177,15 +14024,6 @@
       <c r="F219" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G219" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="H219" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I219" s="1" t="s">
-        <v>895</v>
-      </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C220" s="1" t="s">
@@ -14246,15 +14084,6 @@
       <c r="F222" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G222" s="1" t="s">
-        <v>907</v>
-      </c>
-      <c r="H222" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I222" s="1" t="s">
-        <v>895</v>
-      </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C223" s="1" t="s">
@@ -14268,15 +14097,6 @@
       </c>
       <c r="F223" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="G223" s="1" t="s">
-        <v>908</v>
-      </c>
-      <c r="H223" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I223" s="1" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
@@ -14338,7 +14158,7 @@
   <dimension ref="A1:J229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14352,7 +14172,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1" s="4" t="s">
         <v>378</v>
       </c>
@@ -14372,12 +14192,12 @@
         <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -14389,7 +14209,7 @@
         <v>658</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>387</v>
@@ -14401,18 +14221,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>658</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>382</v>
@@ -14424,18 +14244,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>658</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>383</v>
@@ -14447,18 +14267,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>384</v>
@@ -14470,18 +14290,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>385</v>
@@ -14493,18 +14313,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>733</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>386</v>
@@ -14516,18 +14336,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>600</v>
@@ -14539,18 +14359,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>623</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>897</v>
@@ -14562,18 +14382,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>80</v>
@@ -14585,9 +14405,9 @@
         <v>886</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>843</v>
@@ -14596,10 +14416,10 @@
         <v>529</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>97</v>
@@ -14607,22 +14427,19 @@
       <c r="I11" s="1" t="s">
         <v>886</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>529</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>82</v>
@@ -14634,18 +14451,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>733</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>83</v>
@@ -14657,18 +14474,18 @@
         <v>886</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>733</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>84</v>
@@ -14680,12 +14497,12 @@
         <v>886</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>593</v>
@@ -14703,12 +14520,12 @@
         <v>886</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>593</v>
@@ -14731,7 +14548,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>593</v>
@@ -14754,13 +14571,13 @@
         <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>529</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>88</v>
@@ -14774,16 +14591,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>670</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>161</v>
@@ -14797,16 +14614,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>593</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>109</v>
@@ -14820,16 +14637,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>697</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>102</v>
@@ -14843,16 +14660,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>661</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>103</v>
@@ -14938,7 +14755,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>327</v>
@@ -14947,7 +14764,7 @@
         <v>38</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>97</v>
@@ -14964,7 +14781,7 @@
         <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>593</v>
@@ -14987,13 +14804,13 @@
         <v>641</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>422</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>104</v>
@@ -15010,7 +14827,7 @@
         <v>643</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>325</v>
@@ -15030,19 +14847,19 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>387</v>
@@ -15059,13 +14876,13 @@
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>382</v>
@@ -15082,13 +14899,13 @@
         <v>5</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>529</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>383</v>
@@ -15105,13 +14922,13 @@
         <v>7</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>384</v>
@@ -15128,13 +14945,13 @@
         <v>9</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>385</v>
@@ -15151,13 +14968,13 @@
         <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>386</v>
@@ -15174,13 +14991,13 @@
         <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>600</v>
@@ -15197,13 +15014,13 @@
         <v>623</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1186</v>
+        <v>1180</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>897</v>
@@ -15215,7 +15032,7 @@
         <v>887</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1185</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.2">
@@ -15223,13 +15040,13 @@
         <v>14</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>80</v>
@@ -15243,28 +15060,25 @@
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>702</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>97</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>887</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.2">
@@ -15272,13 +15086,13 @@
         <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>645</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>82</v>
@@ -15295,13 +15109,13 @@
         <v>18</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>83</v>
@@ -15318,13 +15132,13 @@
         <v>20</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>84</v>
@@ -15341,7 +15155,7 @@
         <v>60</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>485</v>
@@ -15364,13 +15178,13 @@
         <v>62</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>86</v>
@@ -15387,13 +15201,13 @@
         <v>64</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>702</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>87</v>
@@ -15410,13 +15224,13 @@
         <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>702</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>88</v>
@@ -15430,16 +15244,16 @@
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>161</v>
@@ -15453,16 +15267,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C49" s="1" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>109</v>
@@ -15476,16 +15290,16 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C50" s="1" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>529</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>102</v>
@@ -15499,16 +15313,16 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C51" s="1" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>700</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>103</v>
@@ -15525,13 +15339,13 @@
         <v>635</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>900</v>
@@ -15603,7 +15417,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>97</v>
@@ -15640,13 +15454,13 @@
         <v>641</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>104</v>
@@ -15663,13 +15477,13 @@
         <v>643</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>105</v>
@@ -15683,19 +15497,19 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>387</v>
@@ -15712,13 +15526,13 @@
         <v>3</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>382</v>
@@ -15735,13 +15549,13 @@
         <v>5</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>383</v>
@@ -15758,13 +15572,13 @@
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>384</v>
@@ -15781,13 +15595,13 @@
         <v>9</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>529</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>385</v>
@@ -15799,18 +15613,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>702</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>386</v>
@@ -15822,18 +15636,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C66" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>702</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>600</v>
@@ -15845,18 +15659,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C67" s="1" t="s">
         <v>623</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>897</v>
@@ -15868,18 +15682,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>80</v>
@@ -15891,21 +15705,21 @@
         <v>888</v>
       </c>
     </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C69" s="1" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>97</v>
@@ -15913,22 +15727,19 @@
       <c r="I69" s="1" t="s">
         <v>888</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C70" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>799</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>82</v>
@@ -15940,9 +15751,9 @@
         <v>888</v>
       </c>
     </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C71" s="1" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>0</v>
@@ -15963,18 +15774,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C72" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>350</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>84</v>
@@ -15986,18 +15797,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C73" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>422</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>85</v>
@@ -16009,18 +15820,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C74" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>86</v>
@@ -16032,18 +15843,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C75" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>422</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>87</v>
@@ -16055,18 +15866,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C76" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>739</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>88</v>
@@ -16078,18 +15889,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C77" s="1" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>161</v>
@@ -16101,18 +15912,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C78" s="1" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>799</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>109</v>
@@ -16124,18 +15935,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C79" s="1" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>799</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>102</v>
@@ -16147,18 +15958,18 @@
         <v>888</v>
       </c>
     </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C80" s="1" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>103</v>
@@ -16175,13 +15986,13 @@
         <v>635</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>670</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>900</v>
@@ -16221,13 +16032,13 @@
         <v>680</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>670</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>898</v>
@@ -16310,13 +16121,13 @@
         <v>643</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>105</v>
@@ -16330,19 +16141,19 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>387</v>
@@ -16359,13 +16170,13 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>382</v>
@@ -16382,13 +16193,13 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>383</v>
@@ -16405,13 +16216,13 @@
         <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>384</v>
@@ -16428,13 +16239,13 @@
         <v>9</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>720</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>385</v>
@@ -16451,13 +16262,13 @@
         <v>11</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>720</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>386</v>
@@ -16474,13 +16285,13 @@
         <v>12</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>600</v>
@@ -16497,13 +16308,13 @@
         <v>14</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>80</v>
@@ -16517,19 +16328,19 @@
     </row>
     <row r="97" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C97" s="1" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>739</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>97</v>
@@ -16543,13 +16354,13 @@
         <v>55</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>799</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>82</v>
@@ -16566,13 +16377,13 @@
         <v>60</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>85</v>
@@ -16589,13 +16400,13 @@
         <v>62</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>86</v>
@@ -16612,13 +16423,13 @@
         <v>64</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>658</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>87</v>
@@ -16635,13 +16446,13 @@
         <v>66</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>88</v>
@@ -16655,16 +16466,16 @@
     </row>
     <row r="103" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C103" s="1" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>700</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>601</v>
@@ -16678,16 +16489,16 @@
     </row>
     <row r="104" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C104" s="1" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>616</v>
@@ -16701,16 +16512,16 @@
     </row>
     <row r="105" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C105" s="1" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>700</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>607</v>
@@ -16724,16 +16535,16 @@
     </row>
     <row r="106" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C106" s="1" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>614</v>
@@ -16750,13 +16561,13 @@
         <v>635</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>900</v>
@@ -16773,13 +16584,13 @@
         <v>637</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>733</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>899</v>
@@ -16796,13 +16607,13 @@
         <v>680</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>733</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>898</v>
@@ -16862,13 +16673,13 @@
         <v>641</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>104</v>
@@ -16885,13 +16696,13 @@
         <v>643</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>733</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>105</v>
@@ -16905,19 +16716,19 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>700</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>387</v>
@@ -16934,13 +16745,13 @@
         <v>3</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>773</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>382</v>
@@ -16957,13 +16768,13 @@
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>383</v>
@@ -16980,13 +16791,13 @@
         <v>7</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>384</v>
@@ -17003,13 +16814,13 @@
         <v>9</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>385</v>
@@ -17026,13 +16837,13 @@
         <v>11</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>386</v>
@@ -17049,13 +16860,13 @@
         <v>12</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>600</v>
@@ -17072,13 +16883,13 @@
         <v>14</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>80</v>
@@ -17092,19 +16903,19 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C123" s="1" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>350</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>97</v>
@@ -17121,13 +16932,13 @@
         <v>55</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>82</v>
@@ -17144,13 +16955,13 @@
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>85</v>
@@ -17167,13 +16978,13 @@
         <v>62</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>86</v>
@@ -17190,13 +17001,13 @@
         <v>64</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>87</v>
@@ -17213,13 +17024,13 @@
         <v>66</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>773</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>88</v>
@@ -17233,16 +17044,16 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C129" s="1" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>601</v>
@@ -17256,16 +17067,16 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C130" s="1" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>616</v>
@@ -17279,16 +17090,16 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C131" s="1" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>741</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>607</v>
@@ -17302,7 +17113,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C132" s="1" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>699</v>
@@ -17311,7 +17122,7 @@
         <v>327</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>614</v>
@@ -17325,19 +17136,19 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C133" s="1" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>370</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>97</v>
@@ -17354,13 +17165,13 @@
         <v>635</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>900</v>
@@ -17377,13 +17188,13 @@
         <v>637</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>899</v>
@@ -17400,13 +17211,13 @@
         <v>680</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>898</v>
@@ -17420,19 +17231,19 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C137" s="1" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>593</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>97</v>
@@ -17443,16 +17254,16 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C138" s="1" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>670</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>97</v>
@@ -17461,7 +17272,7 @@
         <v>890</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
@@ -17512,7 +17323,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>1</v>
@@ -17524,7 +17335,7 @@
         <v>525</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>387</v>
@@ -17541,13 +17352,13 @@
         <v>3</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>741</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>382</v>
@@ -17564,13 +17375,13 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>383</v>
@@ -17587,13 +17398,13 @@
         <v>7</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>384</v>
@@ -17610,13 +17421,13 @@
         <v>9</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>385</v>
@@ -17633,13 +17444,13 @@
         <v>11</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>386</v>
@@ -17656,13 +17467,13 @@
         <v>12</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>600</v>
@@ -17679,13 +17490,13 @@
         <v>623</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>897</v>
@@ -17702,13 +17513,13 @@
         <v>14</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>350</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>80</v>
@@ -17722,7 +17533,7 @@
     </row>
     <row r="151" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C151" s="1" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>0</v>
@@ -17732,12 +17543,6 @@
       </c>
       <c r="F151" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="H151" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I151" s="1" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="152" spans="3:9" x14ac:dyDescent="0.2">
@@ -17753,28 +17558,19 @@
       <c r="F152" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G152" s="1" t="s">
-        <v>903</v>
-      </c>
-      <c r="H152" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I152" s="1" t="s">
-        <v>891</v>
-      </c>
     </row>
     <row r="153" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C153" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>85</v>
@@ -17791,13 +17587,13 @@
         <v>62</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>350</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>86</v>
@@ -17814,13 +17610,13 @@
         <v>64</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>87</v>
@@ -17837,13 +17633,13 @@
         <v>66</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>741</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G156" s="1" t="s">
         <v>88</v>
@@ -17857,16 +17653,16 @@
     </row>
     <row r="157" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C157" s="1" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>350</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>615</v>
@@ -17883,13 +17679,13 @@
         <v>630</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>658</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>108</v>
@@ -17906,13 +17702,13 @@
         <v>715</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>658</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>99</v>
@@ -17926,19 +17722,19 @@
     </row>
     <row r="160" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C160" s="1" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>97</v>
@@ -17949,19 +17745,19 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C161" s="1" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>97</v>
@@ -17978,13 +17774,13 @@
         <v>635</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>670</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="G162" s="1" t="s">
         <v>900</v>
@@ -18024,13 +17820,13 @@
         <v>680</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>670</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>898</v>
@@ -18044,19 +17840,19 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C165" s="1" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="H165" s="1" t="s">
         <v>97</v>
@@ -18067,16 +17863,16 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C166" s="1" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>97</v>
@@ -18085,7 +17881,7 @@
         <v>891</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
@@ -18136,19 +17932,19 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>387</v>
@@ -18165,13 +17961,13 @@
         <v>3</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G171" s="1" t="s">
         <v>382</v>
@@ -18188,13 +17984,13 @@
         <v>5</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>383</v>
@@ -18211,13 +18007,13 @@
         <v>7</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="G173" s="1" t="s">
         <v>384</v>
@@ -18234,13 +18030,13 @@
         <v>9</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>422</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>385</v>
@@ -18257,13 +18053,13 @@
         <v>11</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>386</v>
@@ -18317,7 +18113,7 @@
     </row>
     <row r="178" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C178" s="1" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>0</v>
@@ -18360,13 +18156,13 @@
         <v>60</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G180" s="1" t="s">
         <v>85</v>
@@ -18383,13 +18179,13 @@
         <v>62</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>86</v>
@@ -18406,13 +18202,13 @@
         <v>64</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G182" s="1" t="s">
         <v>87</v>
@@ -18429,13 +18225,13 @@
         <v>66</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>673</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G183" s="1" t="s">
         <v>88</v>
@@ -18449,16 +18245,16 @@
     </row>
     <row r="184" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C184" s="1" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="G184" s="1" t="s">
         <v>615</v>
@@ -18475,13 +18271,13 @@
         <v>630</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>108</v>
@@ -18498,13 +18294,13 @@
         <v>715</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>422</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G186" s="1" t="s">
         <v>403</v>
@@ -18518,19 +18314,19 @@
     </row>
     <row r="187" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C187" s="1" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="H187" s="1" t="s">
         <v>97</v>
@@ -18541,7 +18337,7 @@
     </row>
     <row r="188" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C188" s="1" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>0</v>
@@ -18564,13 +18360,13 @@
         <v>635</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>900</v>
@@ -18587,13 +18383,13 @@
         <v>637</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>899</v>
@@ -18610,13 +18406,13 @@
         <v>680</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>325</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>898</v>
@@ -18630,7 +18426,7 @@
     </row>
     <row r="192" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C192" s="1" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>0</v>
@@ -18650,7 +18446,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C193" s="1" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>0</v>
@@ -18710,19 +18506,19 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G197" s="1" t="s">
         <v>387</v>
@@ -18739,13 +18535,13 @@
         <v>3</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G198" s="1" t="s">
         <v>382</v>
@@ -18762,13 +18558,13 @@
         <v>5</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>383</v>
@@ -18785,13 +18581,13 @@
         <v>7</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>741</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="G200" s="1" t="s">
         <v>384</v>
@@ -18808,13 +18604,13 @@
         <v>9</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>830</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="G201" s="1" t="s">
         <v>385</v>
@@ -18854,13 +18650,13 @@
         <v>12</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="G203" s="1" t="s">
         <v>600</v>
@@ -18877,13 +18673,13 @@
         <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>80</v>
@@ -18923,13 +18719,13 @@
         <v>62</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G206" s="1" t="s">
         <v>86</v>
@@ -18946,13 +18742,13 @@
         <v>64</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G207" s="1" t="s">
         <v>87</v>
@@ -18969,13 +18765,13 @@
         <v>66</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>763</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="G208" s="1" t="s">
         <v>88</v>
@@ -19012,13 +18808,13 @@
         <v>630</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>733</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>108</v>
@@ -19035,13 +18831,13 @@
         <v>751</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="G211" s="1" t="s">
         <v>403</v>
@@ -19058,13 +18854,13 @@
         <v>633</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>652</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="G212" s="1" t="s">
         <v>106</v>
@@ -19078,7 +18874,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C213" s="1" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>0</v>
@@ -19121,13 +18917,13 @@
         <v>637</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>422</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>899</v>
@@ -19144,13 +18940,13 @@
         <v>680</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>485</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>898</v>
@@ -19164,7 +18960,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>1</v>
@@ -19250,13 +19046,13 @@
         <v>9</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>670</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>385</v>
@@ -19373,13 +19169,13 @@
         <v>751</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>525</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="G228" s="1" t="s">
         <v>403</v>

</xml_diff>

<commit_message>
Fixed a couple of U13M results
</commit_message>
<xml_diff>
--- a/2022_CnC_records.xlsx
+++ b/2022_CnC_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5486D378-F7AC-4A1F-AD1F-687B3027D877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47EF84D-A9CC-4142-A348-E3B65F87AD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -5282,7 +5282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E116B990-5FBC-4F60-A519-6D8AF60704F6}">
   <dimension ref="A2:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7337,8 +7337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33EFF66-21E6-4C12-9015-9A2807500A5E}">
   <dimension ref="A2:K89"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8994,7 +8994,7 @@
         <v>428</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>384</v>
+        <v>80</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Fixed a couple of issues in club spreadsheets
</commit_message>
<xml_diff>
--- a/2022_CnC_records.xlsx
+++ b/2022_CnC_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47EF84D-A9CC-4142-A348-E3B65F87AD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF402C-3B90-4C1E-A4C8-D49D4E45BF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4527" uniqueCount="1185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4529" uniqueCount="1187">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2937,9 +2937,6 @@
     <t xml:space="preserve">15:23.2 </t>
   </si>
   <si>
-    <t xml:space="preserve">4:39.5 </t>
-  </si>
-  <si>
     <t xml:space="preserve">21.2 </t>
   </si>
   <si>
@@ -3598,6 +3595,15 @@
   </si>
   <si>
     <t>James Richer</t>
+  </si>
+  <si>
+    <t>CW: this was a 10K road race not track 10000m</t>
+  </si>
+  <si>
+    <t>4:39.54</t>
+  </si>
+  <si>
+    <t>Added 0.04s to match powerof10 time</t>
   </si>
 </sst>
 </file>
@@ -4017,7 +4023,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>376</v>
@@ -4038,7 +4044,7 @@
         <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -4046,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -4593,7 +4599,7 @@
         <v>38</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>97</v>
@@ -4680,7 +4686,7 @@
     </row>
     <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
@@ -5320,7 +5326,7 @@
         <v>95</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -7337,7 +7343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33EFF66-21E6-4C12-9015-9A2807500A5E}">
   <dimension ref="A2:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
@@ -7371,7 +7377,7 @@
         <v>95</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -9017,7 +9023,7 @@
         <v>439</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>97</v>
@@ -9178,7 +9184,7 @@
         <v>306</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>252</v>
@@ -9342,7 +9348,7 @@
   <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9375,7 +9381,7 @@
         <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -9829,7 +9835,7 @@
         <v>662</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>100</v>
@@ -9852,7 +9858,7 @@
         <v>663</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>99</v>
@@ -10071,7 +10077,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>3</v>
       </c>
@@ -10094,7 +10100,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>5</v>
       </c>
@@ -10117,7 +10123,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>7</v>
       </c>
@@ -10140,7 +10146,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>9</v>
       </c>
@@ -10163,7 +10169,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
@@ -10186,7 +10192,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
         <v>12</v>
       </c>
@@ -10209,7 +10215,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
         <v>619</v>
       </c>
@@ -10231,8 +10237,11 @@
       <c r="I39" s="1" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="1" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
         <v>14</v>
       </c>
@@ -10255,7 +10264,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
         <v>673</v>
       </c>
@@ -10269,7 +10278,7 @@
         <v>624</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>98</v>
@@ -10278,7 +10287,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
         <v>55</v>
       </c>
@@ -10301,7 +10310,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
         <v>57</v>
       </c>
@@ -10324,7 +10333,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
         <v>18</v>
       </c>
@@ -10347,7 +10356,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
         <v>60</v>
       </c>
@@ -10370,7 +10379,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
         <v>62</v>
       </c>
@@ -10393,7 +10402,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
         <v>64</v>
       </c>
@@ -10416,7 +10425,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
         <v>66</v>
       </c>
@@ -10913,7 +10922,7 @@
         <v>624</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>98</v>
@@ -11557,7 +11566,7 @@
         <v>743</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>98</v>
@@ -12094,7 +12103,7 @@
         <v>14</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>648</v>
@@ -12112,7 +12121,7 @@
         <v>886</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
@@ -12424,7 +12433,7 @@
         <v>704</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
@@ -14194,8 +14203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA3259E-AFD6-4FCB-BD83-44E5FC56E958}">
   <dimension ref="A1:J229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14229,7 +14238,7 @@
         <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -14456,7 +14465,7 @@
         <v>909</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>97</v>
@@ -14801,7 +14810,7 @@
         <v>38</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>97</v>
@@ -14884,7 +14893,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>1</v>
@@ -15051,7 +15060,7 @@
         <v>619</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>296</v>
@@ -15069,7 +15078,7 @@
         <v>883</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.2">
@@ -15077,7 +15086,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>964</v>
+        <v>1185</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>296</v>
@@ -15093,6 +15102,9 @@
       </c>
       <c r="I39" s="1" t="s">
         <v>883</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>1186</v>
       </c>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
@@ -15100,7 +15112,7 @@
         <v>947</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>698</v>
@@ -15109,7 +15121,7 @@
         <v>948</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>97</v>
@@ -15123,7 +15135,7 @@
         <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>641</v>
@@ -15146,7 +15158,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>296</v>
@@ -15169,7 +15181,7 @@
         <v>20</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>296</v>
@@ -15192,7 +15204,7 @@
         <v>60</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>483</v>
@@ -15215,7 +15227,7 @@
         <v>62</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>662</v>
@@ -15238,7 +15250,7 @@
         <v>64</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>698</v>
@@ -15261,7 +15273,7 @@
         <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>698</v>
@@ -15284,7 +15296,7 @@
         <v>911</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>669</v>
@@ -15307,7 +15319,7 @@
         <v>913</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>669</v>
@@ -15330,7 +15342,7 @@
         <v>950</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>527</v>
@@ -15353,7 +15365,7 @@
         <v>915</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>696</v>
@@ -15454,7 +15466,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>97</v>
@@ -15491,7 +15503,7 @@
         <v>637</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>483</v>
@@ -15514,7 +15526,7 @@
         <v>639</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>483</v>
@@ -15534,19 +15546,19 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>375</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>385</v>
@@ -15563,13 +15575,13 @@
         <v>3</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>375</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>380</v>
@@ -15586,13 +15598,13 @@
         <v>5</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>993</v>
-      </c>
       <c r="F62" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>381</v>
@@ -15609,13 +15621,13 @@
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>382</v>
@@ -15632,13 +15644,13 @@
         <v>9</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>527</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>383</v>
@@ -15655,13 +15667,13 @@
         <v>11</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>698</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>384</v>
@@ -15678,13 +15690,13 @@
         <v>12</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>698</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>596</v>
@@ -15701,13 +15713,13 @@
         <v>619</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>999</v>
-      </c>
       <c r="F67" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>893</v>
@@ -15724,13 +15736,13 @@
         <v>14</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>669</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>80</v>
@@ -15747,7 +15759,7 @@
         <v>947</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>662</v>
@@ -15756,7 +15768,7 @@
         <v>948</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>97</v>
@@ -15770,7 +15782,7 @@
         <v>55</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>795</v>
@@ -15790,7 +15802,7 @@
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C71" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>0</v>
@@ -15816,7 +15828,7 @@
         <v>20</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>348</v>
@@ -15839,13 +15851,13 @@
         <v>60</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>420</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>85</v>
@@ -15862,13 +15874,13 @@
         <v>62</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>375</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>86</v>
@@ -15885,13 +15897,13 @@
         <v>64</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>420</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>87</v>
@@ -15908,7 +15920,7 @@
         <v>66</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>735</v>
@@ -15931,7 +15943,7 @@
         <v>911</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>648</v>
@@ -15954,13 +15966,13 @@
         <v>913</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>795</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>109</v>
@@ -15977,13 +15989,13 @@
         <v>950</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>795</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>102</v>
@@ -16000,7 +16012,7 @@
         <v>915</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>648</v>
@@ -16023,13 +16035,13 @@
         <v>631</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>896</v>
@@ -16069,13 +16081,13 @@
         <v>676</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>894</v>
@@ -16158,13 +16170,13 @@
         <v>639</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>648</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>105</v>
@@ -16178,19 +16190,19 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>669</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>385</v>
@@ -16207,13 +16219,13 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>669</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>380</v>
@@ -16230,13 +16242,13 @@
         <v>5</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>669</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>381</v>
@@ -16253,13 +16265,13 @@
         <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>1032</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>1033</v>
-      </c>
       <c r="F92" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>382</v>
@@ -16276,13 +16288,13 @@
         <v>9</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>716</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>383</v>
@@ -16299,13 +16311,13 @@
         <v>11</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>716</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>384</v>
@@ -16322,13 +16334,13 @@
         <v>12</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>669</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>596</v>
@@ -16345,13 +16357,13 @@
         <v>14</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>669</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>80</v>
@@ -16365,10 +16377,10 @@
     </row>
     <row r="97" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C97" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>735</v>
@@ -16377,7 +16389,7 @@
         <v>948</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>97</v>
@@ -16391,7 +16403,7 @@
         <v>55</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>795</v>
@@ -16414,13 +16426,13 @@
         <v>60</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E99" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>1017</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>1018</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>85</v>
@@ -16437,13 +16449,13 @@
         <v>62</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>669</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>86</v>
@@ -16460,13 +16472,13 @@
         <v>64</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>654</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>87</v>
@@ -16483,13 +16495,13 @@
         <v>66</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E102" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>1019</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>1020</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>88</v>
@@ -16503,16 +16515,16 @@
     </row>
     <row r="103" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C103" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>696</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>597</v>
@@ -16526,16 +16538,16 @@
     </row>
     <row r="104" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C104" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>612</v>
@@ -16549,16 +16561,16 @@
     </row>
     <row r="105" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C105" s="1" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>696</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>603</v>
@@ -16572,10 +16584,10 @@
     </row>
     <row r="106" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C106" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>523</v>
@@ -16598,13 +16610,13 @@
         <v>631</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>759</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>896</v>
@@ -16621,13 +16633,13 @@
         <v>633</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>729</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>895</v>
@@ -16644,13 +16656,13 @@
         <v>676</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>729</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>894</v>
@@ -16710,13 +16722,13 @@
         <v>637</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>483</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>104</v>
@@ -16733,13 +16745,13 @@
         <v>639</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>729</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>105</v>
@@ -16753,13 +16765,13 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>696</v>
@@ -16782,7 +16794,7 @@
         <v>3</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>769</v>
@@ -16805,13 +16817,13 @@
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>381</v>
@@ -16828,13 +16840,13 @@
         <v>7</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>382</v>
@@ -16851,13 +16863,13 @@
         <v>9</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>383</v>
@@ -16874,13 +16886,13 @@
         <v>11</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>483</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>384</v>
@@ -16897,13 +16909,13 @@
         <v>12</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>596</v>
@@ -16920,13 +16932,13 @@
         <v>14</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>483</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>80</v>
@@ -16940,19 +16952,19 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C123" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>348</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>97</v>
@@ -16969,13 +16981,13 @@
         <v>55</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>82</v>
@@ -16992,13 +17004,13 @@
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>85</v>
@@ -17015,13 +17027,13 @@
         <v>62</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>296</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>86</v>
@@ -17038,13 +17050,13 @@
         <v>64</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>648</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>87</v>
@@ -17061,7 +17073,7 @@
         <v>66</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>769</v>
@@ -17081,16 +17093,16 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C129" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>296</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>597</v>
@@ -17104,16 +17116,16 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C130" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>612</v>
@@ -17127,16 +17139,16 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C131" s="1" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>737</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>603</v>
@@ -17150,7 +17162,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C132" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>695</v>
@@ -17159,7 +17171,7 @@
         <v>325</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>610</v>
@@ -17173,19 +17185,19 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C133" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>368</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>97</v>
@@ -17202,13 +17214,13 @@
         <v>631</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>648</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>896</v>
@@ -17225,13 +17237,13 @@
         <v>633</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>296</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>895</v>
@@ -17248,13 +17260,13 @@
         <v>676</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>296</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>894</v>
@@ -17268,19 +17280,19 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C137" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D137" s="1" t="s">
         <v>1061</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>1062</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>589</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>97</v>
@@ -17291,16 +17303,16 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C138" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>1063</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>1064</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>97</v>
@@ -17309,7 +17321,7 @@
         <v>886</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
@@ -17360,7 +17372,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>1</v>
@@ -17372,7 +17384,7 @@
         <v>523</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>385</v>
@@ -17389,7 +17401,7 @@
         <v>3</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>737</v>
@@ -17412,13 +17424,13 @@
         <v>5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>662</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>381</v>
@@ -17435,13 +17447,13 @@
         <v>7</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>662</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>382</v>
@@ -17458,13 +17470,13 @@
         <v>9</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>383</v>
@@ -17481,13 +17493,13 @@
         <v>11</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>384</v>
@@ -17504,13 +17516,13 @@
         <v>12</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>596</v>
@@ -17527,13 +17539,13 @@
         <v>619</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>893</v>
@@ -17550,13 +17562,13 @@
         <v>14</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>348</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>80</v>
@@ -17570,7 +17582,7 @@
     </row>
     <row r="151" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C151" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>0</v>
@@ -17601,13 +17613,13 @@
         <v>60</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>85</v>
@@ -17624,13 +17636,13 @@
         <v>62</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>348</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>86</v>
@@ -17647,13 +17659,13 @@
         <v>64</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>87</v>
@@ -17670,7 +17682,7 @@
         <v>66</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>737</v>
@@ -17690,16 +17702,16 @@
     </row>
     <row r="157" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C157" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>348</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>611</v>
@@ -17716,13 +17728,13 @@
         <v>626</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>654</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>108</v>
@@ -17739,13 +17751,13 @@
         <v>711</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>654</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>99</v>
@@ -17759,19 +17771,19 @@
     </row>
     <row r="160" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C160" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>375</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>97</v>
@@ -17782,19 +17794,19 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C161" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>375</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>97</v>
@@ -17811,13 +17823,13 @@
         <v>631</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G162" s="1" t="s">
         <v>896</v>
@@ -17857,13 +17869,13 @@
         <v>676</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>894</v>
@@ -17877,19 +17889,19 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C165" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>375</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="H165" s="1" t="s">
         <v>97</v>
@@ -17900,16 +17912,16 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C166" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>375</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>97</v>
@@ -17918,7 +17930,7 @@
         <v>887</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
@@ -17969,13 +17981,13 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>375</v>
@@ -17998,7 +18010,7 @@
         <v>3</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>375</v>
@@ -18021,7 +18033,7 @@
         <v>5</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>375</v>
@@ -18044,13 +18056,13 @@
         <v>7</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>483</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="G173" s="1" t="s">
         <v>382</v>
@@ -18067,13 +18079,13 @@
         <v>9</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>420</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>383</v>
@@ -18090,13 +18102,13 @@
         <v>11</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>483</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>384</v>
@@ -18150,7 +18162,7 @@
     </row>
     <row r="178" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C178" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>0</v>
@@ -18193,7 +18205,7 @@
         <v>60</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>375</v>
@@ -18216,7 +18228,7 @@
         <v>62</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>375</v>
@@ -18239,7 +18251,7 @@
         <v>64</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>669</v>
@@ -18262,7 +18274,7 @@
         <v>66</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>669</v>
@@ -18282,16 +18294,16 @@
     </row>
     <row r="184" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C184" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="G184" s="1" t="s">
         <v>611</v>
@@ -18308,13 +18320,13 @@
         <v>626</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>108</v>
@@ -18331,7 +18343,7 @@
         <v>711</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>420</v>
@@ -18351,19 +18363,19 @@
     </row>
     <row r="187" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C187" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="H187" s="1" t="s">
         <v>97</v>
@@ -18374,7 +18386,7 @@
     </row>
     <row r="188" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C188" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>0</v>
@@ -18397,13 +18409,13 @@
         <v>631</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>896</v>
@@ -18420,13 +18432,13 @@
         <v>633</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>895</v>
@@ -18443,13 +18455,13 @@
         <v>676</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>323</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>894</v>
@@ -18463,7 +18475,7 @@
     </row>
     <row r="192" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C192" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>0</v>
@@ -18483,7 +18495,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C193" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>0</v>
@@ -18543,13 +18555,13 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>759</v>
@@ -18572,7 +18584,7 @@
         <v>3</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>648</v>
@@ -18595,7 +18607,7 @@
         <v>5</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>759</v>
@@ -18618,13 +18630,13 @@
         <v>7</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>737</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G200" s="1" t="s">
         <v>382</v>
@@ -18641,13 +18653,13 @@
         <v>9</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>826</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G201" s="1" t="s">
         <v>383</v>
@@ -18687,13 +18699,13 @@
         <v>12</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="G203" s="1" t="s">
         <v>596</v>
@@ -18710,13 +18722,13 @@
         <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>648</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>80</v>
@@ -18779,7 +18791,7 @@
         <v>64</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>759</v>
@@ -18802,7 +18814,7 @@
         <v>66</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>759</v>
@@ -18845,13 +18857,13 @@
         <v>626</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>729</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>108</v>
@@ -18868,13 +18880,13 @@
         <v>747</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>296</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="G211" s="1" t="s">
         <v>401</v>
@@ -18891,13 +18903,13 @@
         <v>629</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>648</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G212" s="1" t="s">
         <v>106</v>
@@ -18911,7 +18923,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C213" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>0</v>
@@ -18954,13 +18966,13 @@
         <v>633</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>420</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>895</v>
@@ -18977,13 +18989,13 @@
         <v>676</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>483</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>894</v>
@@ -18997,7 +19009,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>1</v>
@@ -19083,13 +19095,13 @@
         <v>9</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>666</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>383</v>
@@ -19206,13 +19218,13 @@
         <v>747</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="G228" s="1" t="s">
         <v>401</v>

</xml_diff>